<commit_message>
Refactor place of the class things
</commit_message>
<xml_diff>
--- a/Planning/DefiningModel.xlsx
+++ b/Planning/DefiningModel.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="40">
   <si>
     <t xml:space="preserve">One Generator </t>
   </si>
@@ -105,6 +106,45 @@
   </si>
   <si>
     <t>ExistInFielList</t>
+  </si>
+  <si>
+    <t>One Class Info Data</t>
+  </si>
+  <si>
+    <t>Class Name</t>
+  </si>
+  <si>
+    <t>List of String with LoadedClass</t>
+  </si>
+  <si>
+    <t>SpecificType</t>
+  </si>
+  <si>
+    <t>Class Path</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Template Directory</t>
+  </si>
+  <si>
+    <t>AuthorizationDirectory</t>
+  </si>
+  <si>
+    <t>ViewsDirectory</t>
+  </si>
+  <si>
+    <t>WebMainDirectory</t>
+  </si>
+  <si>
+    <t>WebDirectory, etc</t>
+  </si>
+  <si>
+    <t>Colletions of Items To Replace</t>
+  </si>
+  <si>
+    <t>One Colletions of Config</t>
   </si>
 </sst>
 </file>
@@ -128,7 +168,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -268,11 +308,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -280,6 +333,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -291,17 +358,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -584,8 +647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,11 +671,11 @@
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="9"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="19"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="4"/>
@@ -630,227 +693,227 @@
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="11"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="8"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="14"/>
-      <c r="C7" s="6" t="s">
+      <c r="B7" s="11"/>
+      <c r="C7" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="15"/>
+      <c r="D7" s="16"/>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="11" t="s">
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="8" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="11" t="s">
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="11" t="s">
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="11" t="s">
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="8"/>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="14"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="13"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="10"/>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="4"/>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="15"/>
+      <c r="D14" s="16"/>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="4"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="11" t="s">
+      <c r="C15" s="11"/>
+      <c r="D15" s="8" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="4"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="11" t="s">
+      <c r="C16" s="11"/>
+      <c r="D16" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="4"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="8"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="4"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="13"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="10"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="4"/>
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="18"/>
+      <c r="D19" s="14"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="4"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="11" t="s">
+      <c r="C20" s="11"/>
+      <c r="D20" s="8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="4"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="11" t="s">
+      <c r="C21" s="11"/>
+      <c r="D21" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="4"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="11" t="s">
+      <c r="C22" s="11"/>
+      <c r="D22" s="8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="4"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="8"/>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="4"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="13"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="10"/>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="4"/>
-      <c r="C25" s="17" t="s">
+      <c r="C25" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="18"/>
+      <c r="D25" s="14"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="4"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="11" t="s">
+      <c r="C26" s="11"/>
+      <c r="D26" s="8" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="4"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="11" t="s">
+      <c r="C27" s="11"/>
+      <c r="D27" s="8" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="4"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="8"/>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="4"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="8"/>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="4"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="8"/>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" s="4"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="8"/>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" s="4"/>
-      <c r="C32" s="16"/>
-      <c r="D32" s="13"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="10"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="4"/>
-      <c r="C33" s="10" t="s">
+      <c r="C33" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D33" s="11"/>
+      <c r="D33" s="8"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" s="4"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="11" t="s">
+      <c r="C34" s="7"/>
+      <c r="D34" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" s="4"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="11" t="s">
+      <c r="C35" s="7"/>
+      <c r="D35" s="8" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="4"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="11" t="s">
+      <c r="C36" s="7"/>
+      <c r="D36" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" s="4"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="11" t="s">
+      <c r="C37" s="7"/>
+      <c r="D37" s="8" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" s="4"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="11" t="s">
+      <c r="C38" s="7"/>
+      <c r="D38" s="8" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" s="4"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="11" t="s">
+      <c r="C39" s="7"/>
+      <c r="D39" s="8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" s="4"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="11"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="8"/>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" s="5"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="13"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -860,4 +923,411 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1"/>
+    <col min="4" max="4" width="32.28515625" customWidth="1"/>
+    <col min="5" max="5" width="35.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="11"/>
+      <c r="C4" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="18"/>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="11"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="11"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="11"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="8"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="11"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="8"/>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="11"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="10"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="11"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="10"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="11"/>
+      <c r="C21" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="18"/>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="11"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="14"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="11"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" s="8"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="11"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="8"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="11"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E25" s="8"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="11"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="E26" s="8"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="11"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" s="8"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="11"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="E28" s="8"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="11"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="4"/>
+      <c r="C30" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30" s="18"/>
+      <c r="E30" s="3"/>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="4"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" s="14"/>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="4"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" s="10"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="4"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="8"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="4"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="10"/>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="4"/>
+      <c r="C35" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" s="3"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="4"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E36" s="14"/>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37" s="4"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37" s="10"/>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38" s="4"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="8"/>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39" s="4"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="8"/>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B40" s="4"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="8"/>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B41" s="4"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="8"/>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B42" s="4"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="10"/>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B43" s="4"/>
+      <c r="C43" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D43" s="2"/>
+      <c r="E43" s="3"/>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B44" s="4"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E44" s="14"/>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B45" s="4"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E45" s="8"/>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B46" s="4"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E46" s="8"/>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B47" s="4"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E47" s="8"/>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B48" s="4"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E48" s="8"/>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B49" s="4"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E49" s="10"/>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B50" s="4"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="8"/>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B51" s="5"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C21:D21"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>